<commit_message>
Finish until table Requisito_horario
</commit_message>
<xml_diff>
--- a/db/Curso.xlsx
+++ b/db/Curso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Posgrado\Proyecto Titulacion\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosGrado\Proyecto Titulacion\Timetabling\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A779E94E-B286-4408-9041-098390FB339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3104ED65-DA6D-4EB9-982F-79C83ABF0559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF92CB84-5E73-48F7-873C-5BA243B34C6E}"/>
+    <workbookView xWindow="3345" yWindow="5055" windowWidth="28785" windowHeight="15345" xr2:uid="{BF92CB84-5E73-48F7-873C-5BA243B34C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -210,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,15 +576,15 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -608,7 +606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -619,7 +617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -630,7 +628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -641,7 +639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -652,7 +650,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -663,7 +661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -674,7 +672,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -685,7 +683,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -696,7 +694,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -707,7 +705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -718,7 +716,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -729,7 +727,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -740,7 +738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -751,7 +749,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -762,7 +760,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -773,7 +771,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -784,7 +782,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -795,7 +793,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -806,7 +804,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -817,7 +815,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -828,7 +826,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -839,7 +837,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -850,7 +848,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>50</v>
       </c>

</xml_diff>